<commit_message>
update lunch model example
</commit_message>
<xml_diff>
--- a/Examples/AHP_Lunch/lunchModel_Excel_filledIn.xlsx
+++ b/Examples/AHP_Lunch/lunchModel_Excel_filledIn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitCODE\cdfAHPANPLib\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/AHP_Lunch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF88B030-4DD5-4217-B9B2-398A0693D832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10894AC0-FF47-0A44-A9BA-C7B3FD96C6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1785" windowWidth="12000" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14480" yWindow="540" windowWidth="14320" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise_comp" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>GoalNode</t>
   </si>
   <si>
-    <t>Enter judgments for the paiwise comparisons in the matrix or direct values in the green cells</t>
-  </si>
-  <si>
     <t>2Criteria</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>3Piada</t>
+  </si>
+  <si>
+    <t>Enter pairwise comparisons in the white cells of the table or numerical data in the green cells. For the Direct Values column, if the smallest value is best, invert the value before entering it (e.g., $10 as =1/10) .</t>
   </si>
 </sst>
 </file>
@@ -572,54 +572,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.7109375" customWidth="1"/>
+    <col min="1" max="21" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -643,9 +643,9 @@
         <v>0.37944664031620551</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10">
         <f>1/C4</f>
@@ -670,9 +670,9 @@
         <v>0.18972332015810275</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10">
         <f>1/D4</f>
@@ -698,9 +698,9 @@
         <v>0.22529644268774701</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10">
         <f>1/E4</f>
@@ -727,9 +727,9 @@
         <v>0.20553359683794467</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="12">
         <f>SUM(B4:B7)</f>
@@ -752,51 +752,51 @@
         <v>21.083333333333336</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G9" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="12">
         <f>((MMULT(B8:E8,H4:H7)-4)/(4-1))/0.89</f>
         <v>0.32567985670086319</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="F12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -818,9 +818,9 @@
         <v>0.16176470588235295</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="10">
         <f>1/C13</f>
@@ -842,9 +842,9 @@
         <v>0.44117647058823534</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10">
         <f>1/D13</f>
@@ -867,9 +867,9 @@
         <v>0.3970588235294118</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="12">
         <f>SUM(B13:B15)</f>
@@ -888,51 +888,51 @@
         <v>11.333333333333332</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F17" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="12">
         <f>((MMULT(B16:D16,G13:G15)-3)/(3-1))/0.52</f>
         <v>0.16968325791855229</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -951,9 +951,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="10" t="e">
         <f>1/C21</f>
@@ -976,9 +976,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="10" t="e">
         <f>1/D21</f>
@@ -1004,9 +1004,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="12" t="e">
         <f>SUM(B21:B23)</f>
@@ -1025,51 +1025,51 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F25" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="12" t="e">
         <f>((MMULT(B24:D24,G21:G23)-3)/(3-1))/0.52</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
@@ -1090,9 +1090,9 @@
         <v>9.1869060190073931E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="10">
         <f>1/C29</f>
@@ -1114,9 +1114,9 @@
         <v>0.50686378035902857</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="10">
         <f>1/D29</f>
@@ -1139,9 +1139,9 @@
         <v>0.40126715945089758</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" s="12">
         <f>SUM(B29:B31)</f>
@@ -1160,51 +1160,51 @@
         <v>15.783333333333331</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F33" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33" s="12">
         <f>((MMULT(B32:D32,G29:G31)-3)/(3-1))/0.52</f>
         <v>0.39091056778490785</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="G36" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B37" s="6">
         <v>1</v>
@@ -1225,9 +1225,9 @@
         <v>0.55384615384615388</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B38" s="10">
         <f>1/C37</f>
@@ -1249,9 +1249,9 @@
         <v>0.21538461538461537</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" s="10">
         <f>1/D37</f>
@@ -1274,9 +1274,9 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="12">
         <f>SUM(B37:B39)</f>
@@ -1295,9 +1295,9 @@
         <v>10.833333333333332</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F41" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G41" s="12">
         <f>((MMULT(B40:D40,G37:G39)-3)/(3-1))/0.52</f>

</xml_diff>